<commit_message>
DocumentTypes and NewFieldsForDashboard Done
</commit_message>
<xml_diff>
--- a/src/test/results/TestResults.xlsx
+++ b/src/test/results/TestResults.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="8">
   <si>
     <t>User adds, edits and deletes data in the Position Management functionality</t>
   </si>
@@ -29,6 +29,21 @@
   </si>
   <si>
     <t>User adds, edits and deletes data in the Attestations functionality</t>
+  </si>
+  <si>
+    <t>Add position</t>
+  </si>
+  <si>
+    <t>FAILED</t>
+  </si>
+  <si>
+    <t>Add position in Document Types</t>
+  </si>
+  <si>
+    <t>User adds, edits and deletes in Fields</t>
+  </si>
+  <si>
+    <t>Add position in Fields</t>
   </si>
 </sst>
 </file>
@@ -888,7 +903,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -910,6 +925,502 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>7</v>
+      </c>
+      <c r="B43" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>7</v>
+      </c>
+      <c r="B45" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>7</v>
+      </c>
+      <c r="B46" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>7</v>
+      </c>
+      <c r="B47" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>7</v>
+      </c>
+      <c r="B48" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>7</v>
+      </c>
+      <c r="B49" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>7</v>
+      </c>
+      <c r="B50" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>7</v>
+      </c>
+      <c r="B51" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>7</v>
+      </c>
+      <c r="B52" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>5</v>
+      </c>
+      <c r="B53" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>5</v>
+      </c>
+      <c r="B54" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>5</v>
+      </c>
+      <c r="B55" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>5</v>
+      </c>
+      <c r="B56" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>5</v>
+      </c>
+      <c r="B57" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>5</v>
+      </c>
+      <c r="B58" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>5</v>
+      </c>
+      <c r="B59" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>5</v>
+      </c>
+      <c r="B60" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>5</v>
+      </c>
+      <c r="B61" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>5</v>
+      </c>
+      <c r="B62" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>2</v>
+      </c>
+      <c r="B63" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>5</v>
+      </c>
+      <c r="B64" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>